<commit_message>
Test Extraction on Git ✨
</commit_message>
<xml_diff>
--- a/dataset/xlsx/area.xlsx
+++ b/dataset/xlsx/area.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="61">
   <si>
     <t>Date</t>
   </si>
@@ -43,21 +43,12 @@
     <t>Update</t>
   </si>
   <si>
-    <t>11 มีนาคม 2563</t>
-  </si>
-  <si>
     <t>27 มีนาคม - 10 เมษายน 2563</t>
   </si>
   <si>
-    <t>17-25 มีนาคม 2563</t>
-  </si>
-  <si>
     <t>29 มีนาคม 2563</t>
   </si>
   <si>
-    <t>26 มีนาคม 2563 , 27 มีนาคม 2563</t>
-  </si>
-  <si>
     <t>29 มีนาคม 2563 , 30 มีนาคม 2563</t>
   </si>
   <si>
@@ -73,27 +64,9 @@
     <t>28 มีนาคม 2563</t>
   </si>
   <si>
-    <t>23 กุมภาพันธ์ -  26 มีนาคม 2563</t>
-  </si>
-  <si>
-    <t>15.30-17.00 น.</t>
-  </si>
-  <si>
-    <t>15.00-15.30 น.</t>
-  </si>
-  <si>
-    <t>13.30-14.55 น.</t>
-  </si>
-  <si>
-    <t>16.00-20.00 น.</t>
-  </si>
-  <si>
     <t>07.55 น.</t>
   </si>
   <si>
-    <t>19.20 น. , 05.00 น.</t>
-  </si>
-  <si>
     <t>12.34 น. , 06.00 น.</t>
   </si>
   <si>
@@ -112,27 +85,12 @@
     <t>17.00 น.</t>
   </si>
   <si>
-    <t>ผู้โดยสารรถตู้หนานคำ สถานีขนส่งเชียงราย 2 – สถานีขนส่งแพร่</t>
-  </si>
-  <si>
-    <t>ผู้โดยสารรถโดยสารประจำทางสนามบินแม่ฟ้าหลวง – สถานีขนส่งเชียงราย 2</t>
-  </si>
-  <si>
-    <t>ผู้ที่เดินทางสายการบิน  VietjetAir เที่ยวบิน VZ132 เส้นทาง สุวรรณภูมิ - เชียงราย (แม่ฟ้าหลวง)</t>
-  </si>
-  <si>
     <t>ซอยบางลา ต.ป่าตอง อ.กะทู้</t>
   </si>
   <si>
-    <t>ตลาดหน้าโวคท หัวรั้ว อ.หาดใหญ่ ระหว่างร้านขายปลาเผาและขายลอตเตอรี่</t>
-  </si>
-  <si>
     <t>ผู้โดยสารสายการบินนกแอร์ เที่ยวบินที่ DD7103 เส้นทางหาดใหญ่ - ดอนเมือง เลขที่นั่ง 34A (ติดตามผู้สัมผัสใกล้ชิด 2 แถวหน้า-หลังครบแล้ว เว้นที่นั่ง 34A)</t>
   </si>
   <si>
-    <t>ขอความร่วมมือผู้ที่โดยสารรถประจำทาง นครชัยแอร์ เส้นทาง ระยอง - อุบลราชธานี เลขรถ 588-276-BF ถึงศรีสะเกษ</t>
-  </si>
-  <si>
     <t>ผู้โดยสารสายการบินไทย เที่ยวบิน TG911 เส้นทาง ประเทศอังกฤษ - สุวรรณภูมิ เลขที่นั่ง 45K 44H 44K 45H</t>
   </si>
   <si>
@@ -157,21 +115,12 @@
     <t>ผู้ที่เดินทางสายการบิน KLM เที่ยวบินที่ 0875 เส้นทาง อัมสเตอร์อัม - สุวรรณภูมิ ทุกแถว (ยกเว้นแถวที่ 20-24)</t>
   </si>
   <si>
-    <t>สถานประกอบการ บาร์เบียร์ ซอย 6 พัทยา</t>
-  </si>
-  <si>
-    <t>สำนักงานสาธารณสุขจังหวัดเชียงราย 8 เมษายน 2563</t>
-  </si>
-  <si>
     <t>สำนักงานสาธารณสุขจังหวัดภูเก็ต 27 มีนาคม 2563</t>
   </si>
   <si>
     <t>สำนักงานสาธารณสุขจังหวัดสงขลา  4 เมษายน 2563</t>
   </si>
   <si>
-    <t>สำนักงานสาธารณสุขจังหวัดศรีสะเกษ 4 เมษายน 2563</t>
-  </si>
-  <si>
     <t>สำนักงานสาธารณสุขจังหวัดปราจีนนบุรี 4 เมษายน 2563</t>
   </si>
   <si>
@@ -184,21 +133,12 @@
     <t>ศูนย์ปฏิบัติการตอบโต้ภาวะฉุกเฉิน โรคติดเชื้อไวรัสโคโรนา 2019 จังหวัดอุบลราชธานี 1 เมษายน 2563</t>
   </si>
   <si>
-    <t>คณะกรรมการโรคติดต่อจังหวัดชลบุรี27 มีนาคม 2563</t>
-  </si>
-  <si>
-    <t>เชียงราย</t>
-  </si>
-  <si>
     <t>ภูเก็ต</t>
   </si>
   <si>
     <t>สงขลา</t>
   </si>
   <si>
-    <t>ศรีสะเกษ</t>
-  </si>
-  <si>
     <t>ปราจีนบุรี</t>
   </si>
   <si>
@@ -211,21 +151,12 @@
     <t>อุบลราชธานี</t>
   </si>
   <si>
-    <t>ชลบุรี</t>
-  </si>
-  <si>
-    <t>Chiang Rai</t>
-  </si>
-  <si>
     <t>Phuket</t>
   </si>
   <si>
     <t>Songkhla</t>
   </si>
   <si>
-    <t>Sisaket</t>
-  </si>
-  <si>
     <t>Prachinburi</t>
   </si>
   <si>
@@ -238,30 +169,12 @@
     <t>Ubon Ratchathani</t>
   </si>
   <si>
-    <t>Chonburi</t>
-  </si>
-  <si>
-    <t>2020-04-08 12:13:34</t>
-  </si>
-  <si>
-    <t>2020-04-08 12:10:50</t>
-  </si>
-  <si>
-    <t>2020-04-08 12:08:31</t>
-  </si>
-  <si>
     <t>2020-04-08 11:58:58</t>
   </si>
   <si>
-    <t>2020-04-08 06:41:45</t>
-  </si>
-  <si>
     <t>2020-04-08 06:37:16</t>
   </si>
   <si>
-    <t>2020-04-08 06:25:42</t>
-  </si>
-  <si>
     <t>2020-04-08 06:11:43</t>
   </si>
   <si>
@@ -284,9 +197,6 @@
   </si>
   <si>
     <t>2020-04-03 13:26:17</t>
-  </si>
-  <si>
-    <t>2020-03-31 08:58:45</t>
   </si>
 </sst>
 </file>
@@ -644,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I17"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -683,362 +593,227 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>33</v>
       </c>
       <c r="G2" t="s">
-        <v>57</v>
+        <v>39</v>
       </c>
       <c r="H2" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="I2" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="G3" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="H5" t="s">
-        <v>67</v>
+        <v>48</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" t="s">
         <v>36</v>
       </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
       <c r="G6" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" t="s">
         <v>37</v>
       </c>
-      <c r="F7" t="s">
-        <v>50</v>
-      </c>
       <c r="G7" t="s">
-        <v>59</v>
+        <v>43</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="F8" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="G8" t="s">
-        <v>60</v>
+        <v>43</v>
       </c>
       <c r="H8" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="I8" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F9" t="s">
-        <v>52</v>
+        <v>37</v>
       </c>
       <c r="G9" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="H9" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="I9" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="F10" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="G10" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="H10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="I10" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="H11" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
-      <c r="A12" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G12" t="s">
-        <v>63</v>
-      </c>
-      <c r="H12" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" t="s">
-        <v>54</v>
-      </c>
-      <c r="G13" t="s">
-        <v>63</v>
-      </c>
-      <c r="H13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I13" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I14" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" t="s">
-        <v>64</v>
-      </c>
-      <c r="H15" t="s">
-        <v>73</v>
-      </c>
-      <c r="I15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" t="s">
-        <v>55</v>
-      </c>
-      <c r="G16" t="s">
-        <v>64</v>
-      </c>
-      <c r="H16" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" t="s">
-        <v>56</v>
-      </c>
-      <c r="G17" t="s">
-        <v>65</v>
-      </c>
-      <c r="H17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" t="s">
-        <v>90</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Extraction on Git ✨ ศ. 15 เม.ย. 63 เวลา 03:17
</commit_message>
<xml_diff>
--- a/dataset/xlsx/area.xlsx
+++ b/dataset/xlsx/area.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Date</t>
   </si>
@@ -46,64 +46,19 @@
     <t>27 มีนาคม - 10 เมษายน 2563</t>
   </si>
   <si>
-    <t>30 มีนาคม 2563</t>
-  </si>
-  <si>
-    <t>14.30 น.</t>
-  </si>
-  <si>
-    <t>12.20 น.</t>
-  </si>
-  <si>
     <t>ซอยบางลา ต.ป่าตอง อ.กะทู้</t>
   </si>
   <si>
-    <t>ผู้โดยสารรถตู้ คันที่ 17 ทะเบียน 10-0251 จากสถานีขนส่งอุบลราชธานี - อำนาจเจริญ (ทุกคน)</t>
-  </si>
-  <si>
-    <t>ผู้ที่เดินทางสายการบิน ไทยสไมล์ เที่ยวบิน WE024 เส้นทาง สุวรรณภูมิ - อุบลราชธานี แถวที่ 46-50</t>
-  </si>
-  <si>
-    <t>ผู้ที่เดินทางสายการบิน ไทยสไมล์ เที่ยวบิน WE024 เส้นทาง สุวรรณภูมิ - อุบลราชธานี ทุกแถว (ยกเว้นแถวที่ 46-50)</t>
-  </si>
-  <si>
     <t>สำนักงานสาธารณสุขจังหวัดภูเก็ต 27 มีนาคม 2563</t>
   </si>
   <si>
-    <t>คณะกรรมการโรคติดต่อจังหวัดอำนาจเจริญ 1 เมษายน 2563</t>
-  </si>
-  <si>
-    <t>ศูนย์ปฏิบัติการตอบโต้ภาวะฉุกเฉิน โรคติดเชื้อไวรัสโคโรนา 2019 จังหวัดอุบลราชธานี 1 เมษายน 2563</t>
-  </si>
-  <si>
     <t>ภูเก็ต</t>
   </si>
   <si>
-    <t>อำนาจเจริญ</t>
-  </si>
-  <si>
-    <t>อุบลราชธานี</t>
-  </si>
-  <si>
     <t>Phuket</t>
   </si>
   <si>
-    <t>Amnat Charoen</t>
-  </si>
-  <si>
-    <t>Ubon Ratchathani</t>
-  </si>
-  <si>
     <t>2020-04-12 10:47:44</t>
-  </si>
-  <si>
-    <t>2020-04-03 13:38:42</t>
-  </si>
-  <si>
-    <t>2020-04-03 13:36:39</t>
-  </si>
-  <si>
-    <t>2020-04-03 13:29:12</t>
   </si>
 </sst>
 </file>
@@ -461,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -501,88 +456,19 @@
         <v>9</v>
       </c>
       <c r="D2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>23</v>
-      </c>
       <c r="I2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>24</v>
-      </c>
-      <c r="I3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" t="s">
-        <v>24</v>
-      </c>
-      <c r="I4" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
-      </c>
-      <c r="G5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" t="s">
-        <v>25</v>
-      </c>
-      <c r="I5" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>